<commit_message>
[ADD] Show Task / Issue link on report hours
</commit_message>
<xml_diff>
--- a/report_hours_consumption/static/template/base.xlsx
+++ b/report_hours_consumption/static/template/base.xlsx
@@ -5,14 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet0!$A$4:$K$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet0!$A$4:$K$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -183,7 +182,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -216,18 +215,14 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -237,30 +232,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7044534412956"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.0607287449393"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="40.8137651821862"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.78542510121457"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="40.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="36.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -330,9 +325,10 @@
       <c r="K4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="M4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -413,7 +409,7 @@
   </mergeCells>
   <printOptions headings="true" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>